<commit_message>
Reformat Excel and CSV files
</commit_message>
<xml_diff>
--- a/states.xlsx
+++ b/states.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlessandroDeCarlo\Desktop\DT\RL\Axitinib\RLdbp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0AD9C0-476E-4D98-A756-04BEE9A788FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB9FD44-E304-4E8C-A221-0E6A3DEDEAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5CD8DD80-2877-4D1B-A289-3A5EBDE7C74E}"/>
   </bookViews>
@@ -422,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F34575-0022-41A3-98D8-27B35D0E8796}">
-  <dimension ref="A1:E245"/>
+  <dimension ref="A1:E205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +515,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -526,14 +526,14 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" ref="A6:A69" si="0">A5+1</f>
+        <f t="shared" ref="A6:A68" si="0">A5+1</f>
         <v>5</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -551,7 +551,7 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -587,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -598,17 +598,17 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f>A9+1</f>
         <v>9</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -659,7 +659,7 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -677,7 +677,7 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -695,10 +695,10 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -713,10 +713,10 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -731,7 +731,7 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -749,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -785,10 +785,10 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -803,10 +803,10 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -821,10 +821,10 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -839,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -857,7 +857,7 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -875,10 +875,10 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -893,10 +893,10 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -911,10 +911,10 @@
         <v>1</v>
       </c>
       <c r="C27">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -929,10 +929,10 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -947,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D29">
         <v>4</v>
@@ -968,10 +968,10 @@
         <v>2</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -986,10 +986,10 @@
         <v>3</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1004,10 +1004,10 @@
         <v>5</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1022,10 +1022,10 @@
         <v>7</v>
       </c>
       <c r="D33">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1040,10 +1040,10 @@
         <v>10</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1055,10 +1055,10 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1073,10 +1073,10 @@
         <v>1</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1091,10 +1091,10 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1109,10 +1109,10 @@
         <v>1</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1127,10 +1127,10 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1145,10 +1145,10 @@
         <v>1</v>
       </c>
       <c r="C40">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1163,10 +1163,10 @@
         <v>1</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1181,10 +1181,10 @@
         <v>1</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1199,10 +1199,10 @@
         <v>1</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -1217,10 +1217,10 @@
         <v>1</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1235,10 +1235,10 @@
         <v>1</v>
       </c>
       <c r="C45">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -1253,10 +1253,10 @@
         <v>1</v>
       </c>
       <c r="C46">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1271,10 +1271,10 @@
         <v>1</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1289,10 +1289,10 @@
         <v>1</v>
       </c>
       <c r="C48">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -1307,10 +1307,10 @@
         <v>1</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -1325,10 +1325,10 @@
         <v>1</v>
       </c>
       <c r="C50">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -1343,10 +1343,10 @@
         <v>1</v>
       </c>
       <c r="C51">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -1361,10 +1361,10 @@
         <v>1</v>
       </c>
       <c r="C52">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -1379,10 +1379,10 @@
         <v>1</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -1397,10 +1397,10 @@
         <v>1</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D54">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -1412,16 +1412,16 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D55">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1430,16 +1430,16 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1448,16 +1448,16 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C57">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D57">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1466,16 +1466,16 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C58">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D58">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1484,16 +1484,16 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D59">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1502,16 +1502,16 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C60">
         <v>2</v>
       </c>
       <c r="D60">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1520,16 +1520,16 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C61">
         <v>3</v>
       </c>
       <c r="D61">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -1538,16 +1538,16 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C62">
         <v>5</v>
       </c>
       <c r="D62">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -1556,16 +1556,16 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C63">
         <v>7</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -1574,16 +1574,16 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C64">
         <v>10</v>
       </c>
       <c r="D64">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -1595,10 +1595,10 @@
         <v>2</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -1613,10 +1613,10 @@
         <v>2</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -1631,10 +1631,10 @@
         <v>2</v>
       </c>
       <c r="C67">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -1649,10 +1649,10 @@
         <v>2</v>
       </c>
       <c r="C68">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -1660,17 +1660,17 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A69:A132" si="1">A68+1</f>
         <v>68</v>
       </c>
       <c r="B69">
         <v>2</v>
       </c>
       <c r="C69">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -1678,17 +1678,17 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
-        <f t="shared" ref="A70:A133" si="1">A69+1</f>
+        <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="B70">
         <v>2</v>
       </c>
       <c r="C70">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -1703,10 +1703,10 @@
         <v>2</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -1721,10 +1721,10 @@
         <v>2</v>
       </c>
       <c r="C72">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -1739,10 +1739,10 @@
         <v>2</v>
       </c>
       <c r="C73">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -1757,10 +1757,10 @@
         <v>2</v>
       </c>
       <c r="C74">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -1775,10 +1775,10 @@
         <v>2</v>
       </c>
       <c r="C75">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -1793,10 +1793,10 @@
         <v>2</v>
       </c>
       <c r="C76">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -1811,10 +1811,10 @@
         <v>2</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -1829,10 +1829,10 @@
         <v>2</v>
       </c>
       <c r="C78">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D78">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -1847,10 +1847,10 @@
         <v>2</v>
       </c>
       <c r="C79">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D79">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -1865,13 +1865,13 @@
         <v>2</v>
       </c>
       <c r="C80">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D80">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -1883,13 +1883,13 @@
         <v>2</v>
       </c>
       <c r="C81">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -1901,13 +1901,13 @@
         <v>2</v>
       </c>
       <c r="C82">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D82">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -1919,13 +1919,13 @@
         <v>2</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D83">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -1937,13 +1937,13 @@
         <v>2</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D84">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -1955,13 +1955,13 @@
         <v>2</v>
       </c>
       <c r="C85">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D85">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -1973,13 +1973,13 @@
         <v>2</v>
       </c>
       <c r="C86">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D86">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -1991,13 +1991,13 @@
         <v>2</v>
       </c>
       <c r="C87">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D87">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -2009,13 +2009,13 @@
         <v>2</v>
       </c>
       <c r="C88">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D88">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -2027,13 +2027,13 @@
         <v>2</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D89">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -2048,10 +2048,10 @@
         <v>2</v>
       </c>
       <c r="D90">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -2066,10 +2066,10 @@
         <v>3</v>
       </c>
       <c r="D91">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -2084,10 +2084,10 @@
         <v>5</v>
       </c>
       <c r="D92">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -2102,10 +2102,10 @@
         <v>7</v>
       </c>
       <c r="D93">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -2120,10 +2120,10 @@
         <v>10</v>
       </c>
       <c r="D94">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -2135,10 +2135,10 @@
         <v>2</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -2153,10 +2153,10 @@
         <v>2</v>
       </c>
       <c r="C96">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -2171,10 +2171,10 @@
         <v>2</v>
       </c>
       <c r="C97">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -2189,10 +2189,10 @@
         <v>2</v>
       </c>
       <c r="C98">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E98">
         <v>1</v>
@@ -2207,10 +2207,10 @@
         <v>2</v>
       </c>
       <c r="C99">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -2225,10 +2225,10 @@
         <v>2</v>
       </c>
       <c r="C100">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -2243,10 +2243,10 @@
         <v>2</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -2261,10 +2261,10 @@
         <v>2</v>
       </c>
       <c r="C102">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -2279,10 +2279,10 @@
         <v>2</v>
       </c>
       <c r="C103">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -2297,10 +2297,10 @@
         <v>2</v>
       </c>
       <c r="C104">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E104">
         <v>1</v>
@@ -2312,16 +2312,16 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C105">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -2330,16 +2330,16 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C106">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -2348,16 +2348,16 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D107">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -2366,16 +2366,16 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C108">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D108">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -2384,16 +2384,16 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C109">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D109">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -2402,16 +2402,16 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C110">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D110">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E110">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -2420,16 +2420,16 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C111">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E111">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -2438,16 +2438,16 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C112">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E112">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -2456,16 +2456,16 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D113">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E113">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -2474,16 +2474,16 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C114">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D114">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -2492,16 +2492,16 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C115">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D115">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E115">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -2510,16 +2510,16 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C116">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D116">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -2528,16 +2528,16 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C117">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D117">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -2546,16 +2546,16 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C118">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D118">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
@@ -2564,16 +2564,16 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D119">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E119">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -2582,16 +2582,16 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C120">
         <v>2</v>
       </c>
       <c r="D120">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -2600,16 +2600,16 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C121">
         <v>3</v>
       </c>
       <c r="D121">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
@@ -2618,16 +2618,16 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C122">
         <v>5</v>
       </c>
       <c r="D122">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -2636,16 +2636,16 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C123">
         <v>7</v>
       </c>
       <c r="D123">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
@@ -2654,16 +2654,16 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C124">
         <v>10</v>
       </c>
       <c r="D124">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -2675,10 +2675,10 @@
         <v>3</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E125">
         <v>0</v>
@@ -2693,10 +2693,10 @@
         <v>3</v>
       </c>
       <c r="C126">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E126">
         <v>0</v>
@@ -2711,10 +2711,10 @@
         <v>3</v>
       </c>
       <c r="C127">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E127">
         <v>0</v>
@@ -2729,10 +2729,10 @@
         <v>3</v>
       </c>
       <c r="C128">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E128">
         <v>0</v>
@@ -2747,10 +2747,10 @@
         <v>3</v>
       </c>
       <c r="C129">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E129">
         <v>0</v>
@@ -2765,13 +2765,13 @@
         <v>3</v>
       </c>
       <c r="C130">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D130">
         <v>0</v>
       </c>
       <c r="E130">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -2783,13 +2783,13 @@
         <v>3</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -2801,49 +2801,49 @@
         <v>3</v>
       </c>
       <c r="C132">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D132">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E132">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A133:A196" si="2">A132+1</f>
         <v>132</v>
       </c>
       <c r="B133">
         <v>3</v>
       </c>
       <c r="C133">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
-        <f t="shared" ref="A134:A197" si="2">A133+1</f>
+        <f t="shared" si="2"/>
         <v>133</v>
       </c>
       <c r="B134">
         <v>3</v>
       </c>
       <c r="C134">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E134">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -2855,13 +2855,13 @@
         <v>3</v>
       </c>
       <c r="C135">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D135">
         <v>1</v>
       </c>
       <c r="E135">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -2873,13 +2873,13 @@
         <v>3</v>
       </c>
       <c r="C136">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D136">
         <v>1</v>
       </c>
       <c r="E136">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -2891,13 +2891,13 @@
         <v>3</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D137">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E137">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -2909,13 +2909,13 @@
         <v>3</v>
       </c>
       <c r="C138">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D138">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E138">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -2927,13 +2927,13 @@
         <v>3</v>
       </c>
       <c r="C139">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D139">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -2945,13 +2945,13 @@
         <v>3</v>
       </c>
       <c r="C140">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D140">
         <v>2</v>
       </c>
       <c r="E140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -2963,13 +2963,13 @@
         <v>3</v>
       </c>
       <c r="C141">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D141">
         <v>2</v>
       </c>
       <c r="E141">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -2981,13 +2981,13 @@
         <v>3</v>
       </c>
       <c r="C142">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D142">
         <v>2</v>
       </c>
       <c r="E142">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -2999,13 +2999,13 @@
         <v>3</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D143">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E143">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -3017,13 +3017,13 @@
         <v>3</v>
       </c>
       <c r="C144">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D144">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E144">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -3035,13 +3035,13 @@
         <v>3</v>
       </c>
       <c r="C145">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D145">
         <v>3</v>
       </c>
       <c r="E145">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -3053,13 +3053,13 @@
         <v>3</v>
       </c>
       <c r="C146">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D146">
         <v>3</v>
       </c>
       <c r="E146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -3071,13 +3071,13 @@
         <v>3</v>
       </c>
       <c r="C147">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D147">
         <v>3</v>
       </c>
       <c r="E147">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -3089,13 +3089,13 @@
         <v>3</v>
       </c>
       <c r="C148">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D148">
         <v>3</v>
       </c>
       <c r="E148">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -3107,13 +3107,13 @@
         <v>3</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D149">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -3131,7 +3131,7 @@
         <v>4</v>
       </c>
       <c r="E150">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -3149,7 +3149,7 @@
         <v>4</v>
       </c>
       <c r="E151">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -3167,7 +3167,7 @@
         <v>4</v>
       </c>
       <c r="E152">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -3185,7 +3185,7 @@
         <v>4</v>
       </c>
       <c r="E153">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -3203,7 +3203,7 @@
         <v>4</v>
       </c>
       <c r="E154">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -3212,16 +3212,16 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D155">
         <v>0</v>
       </c>
       <c r="E155">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -3230,16 +3230,16 @@
         <v>155</v>
       </c>
       <c r="B156">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C156">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D156">
         <v>0</v>
       </c>
       <c r="E156">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -3248,16 +3248,16 @@
         <v>156</v>
       </c>
       <c r="B157">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C157">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D157">
         <v>0</v>
       </c>
       <c r="E157">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -3266,16 +3266,16 @@
         <v>157</v>
       </c>
       <c r="B158">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C158">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D158">
         <v>0</v>
       </c>
       <c r="E158">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -3284,16 +3284,16 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C159">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D159">
         <v>0</v>
       </c>
       <c r="E159">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -3302,16 +3302,16 @@
         <v>159</v>
       </c>
       <c r="B160">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C160">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D160">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E160">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
@@ -3320,16 +3320,16 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D161">
         <v>1</v>
       </c>
       <c r="E161">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
@@ -3338,16 +3338,16 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C162">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D162">
         <v>1</v>
       </c>
       <c r="E162">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
@@ -3356,16 +3356,16 @@
         <v>162</v>
       </c>
       <c r="B163">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C163">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D163">
         <v>1</v>
       </c>
       <c r="E163">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
@@ -3374,16 +3374,16 @@
         <v>163</v>
       </c>
       <c r="B164">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C164">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D164">
         <v>1</v>
       </c>
       <c r="E164">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
@@ -3392,16 +3392,16 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C165">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D165">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E165">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
@@ -3410,16 +3410,16 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C166">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D166">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E166">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
@@ -3428,16 +3428,16 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D167">
         <v>2</v>
       </c>
       <c r="E167">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
@@ -3446,16 +3446,16 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C168">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D168">
         <v>2</v>
       </c>
       <c r="E168">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
@@ -3464,16 +3464,16 @@
         <v>168</v>
       </c>
       <c r="B169">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C169">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D169">
         <v>2</v>
       </c>
       <c r="E169">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
@@ -3482,16 +3482,16 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C170">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D170">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E170">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
@@ -3500,16 +3500,16 @@
         <v>170</v>
       </c>
       <c r="B171">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C171">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D171">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E171">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
@@ -3518,16 +3518,16 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C172">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D172">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E172">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
@@ -3536,16 +3536,16 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C173">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D173">
         <v>3</v>
       </c>
       <c r="E173">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
@@ -3554,16 +3554,16 @@
         <v>173</v>
       </c>
       <c r="B174">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C174">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D174">
         <v>3</v>
       </c>
       <c r="E174">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
@@ -3572,16 +3572,16 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C175">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D175">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E175">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
@@ -3590,16 +3590,16 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C176">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D176">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E176">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
@@ -3608,16 +3608,16 @@
         <v>176</v>
       </c>
       <c r="B177">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C177">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D177">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E177">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
@@ -3626,16 +3626,16 @@
         <v>177</v>
       </c>
       <c r="B178">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C178">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D178">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E178">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
@@ -3644,16 +3644,16 @@
         <v>178</v>
       </c>
       <c r="B179">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C179">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D179">
         <v>4</v>
       </c>
       <c r="E179">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
@@ -3662,13 +3662,13 @@
         <v>179</v>
       </c>
       <c r="B180">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C180">
         <v>2</v>
       </c>
       <c r="D180">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E180">
         <v>1</v>
@@ -3680,13 +3680,13 @@
         <v>180</v>
       </c>
       <c r="B181">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C181">
         <v>3</v>
       </c>
       <c r="D181">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E181">
         <v>1</v>
@@ -3698,13 +3698,13 @@
         <v>181</v>
       </c>
       <c r="B182">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C182">
         <v>5</v>
       </c>
       <c r="D182">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E182">
         <v>1</v>
@@ -3716,13 +3716,13 @@
         <v>182</v>
       </c>
       <c r="B183">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C183">
         <v>7</v>
       </c>
       <c r="D183">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E183">
         <v>1</v>
@@ -3734,13 +3734,13 @@
         <v>183</v>
       </c>
       <c r="B184">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C184">
         <v>10</v>
       </c>
       <c r="D184">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E184">
         <v>1</v>
@@ -3755,13 +3755,13 @@
         <v>4</v>
       </c>
       <c r="C185">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D185">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E185">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
@@ -3773,13 +3773,13 @@
         <v>4</v>
       </c>
       <c r="C186">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D186">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E186">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
@@ -3791,13 +3791,13 @@
         <v>4</v>
       </c>
       <c r="C187">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D187">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E187">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
@@ -3809,13 +3809,13 @@
         <v>4</v>
       </c>
       <c r="C188">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D188">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E188">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
@@ -3827,13 +3827,13 @@
         <v>4</v>
       </c>
       <c r="C189">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D189">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E189">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
@@ -3845,13 +3845,13 @@
         <v>4</v>
       </c>
       <c r="C190">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D190">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E190">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
@@ -3863,13 +3863,13 @@
         <v>4</v>
       </c>
       <c r="C191">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D191">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E191">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
@@ -3881,13 +3881,13 @@
         <v>4</v>
       </c>
       <c r="C192">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D192">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E192">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
@@ -3899,13 +3899,13 @@
         <v>4</v>
       </c>
       <c r="C193">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D193">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E193">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
@@ -3917,13 +3917,13 @@
         <v>4</v>
       </c>
       <c r="C194">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D194">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E194">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
@@ -3935,13 +3935,13 @@
         <v>4</v>
       </c>
       <c r="C195">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D195">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E195">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
@@ -3953,49 +3953,49 @@
         <v>4</v>
       </c>
       <c r="C196">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D196">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E196">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A197:A205" si="3">A196+1</f>
         <v>196</v>
       </c>
       <c r="B197">
         <v>4</v>
       </c>
       <c r="C197">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D197">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E197">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198">
-        <f t="shared" ref="A198:A244" si="3">A197+1</f>
+        <f t="shared" si="3"/>
         <v>197</v>
       </c>
       <c r="B198">
         <v>4</v>
       </c>
       <c r="C198">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D198">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E198">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
@@ -4007,13 +4007,13 @@
         <v>4</v>
       </c>
       <c r="C199">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D199">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E199">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
@@ -4025,13 +4025,13 @@
         <v>4</v>
       </c>
       <c r="C200">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D200">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E200">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
@@ -4043,13 +4043,13 @@
         <v>4</v>
       </c>
       <c r="C201">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D201">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E201">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
@@ -4061,13 +4061,13 @@
         <v>4</v>
       </c>
       <c r="C202">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D202">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E202">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
@@ -4079,13 +4079,13 @@
         <v>4</v>
       </c>
       <c r="C203">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D203">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E203">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
@@ -4097,13 +4097,13 @@
         <v>4</v>
       </c>
       <c r="C204">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D204">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E204">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
@@ -4112,734 +4112,15 @@
         <v>204</v>
       </c>
       <c r="B205">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C205">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="D205">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="E205">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A206">
-        <f t="shared" si="3"/>
-        <v>205</v>
-      </c>
-      <c r="B206">
-        <v>4</v>
-      </c>
-      <c r="C206">
-        <v>5</v>
-      </c>
-      <c r="D206">
-        <v>3</v>
-      </c>
-      <c r="E206">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A207">
-        <f t="shared" si="3"/>
-        <v>206</v>
-      </c>
-      <c r="B207">
-        <v>4</v>
-      </c>
-      <c r="C207">
-        <v>7</v>
-      </c>
-      <c r="D207">
-        <v>3</v>
-      </c>
-      <c r="E207">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A208">
-        <f t="shared" si="3"/>
-        <v>207</v>
-      </c>
-      <c r="B208">
-        <v>4</v>
-      </c>
-      <c r="C208">
-        <v>10</v>
-      </c>
-      <c r="D208">
-        <v>3</v>
-      </c>
-      <c r="E208">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A209">
-        <f t="shared" si="3"/>
-        <v>208</v>
-      </c>
-      <c r="B209">
-        <v>4</v>
-      </c>
-      <c r="C209">
-        <v>0</v>
-      </c>
-      <c r="D209">
-        <v>4</v>
-      </c>
-      <c r="E209">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A210">
-        <f t="shared" si="3"/>
-        <v>209</v>
-      </c>
-      <c r="B210">
-        <v>4</v>
-      </c>
-      <c r="C210">
-        <v>2</v>
-      </c>
-      <c r="D210">
-        <v>4</v>
-      </c>
-      <c r="E210">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A211">
-        <f t="shared" si="3"/>
-        <v>210</v>
-      </c>
-      <c r="B211">
-        <v>4</v>
-      </c>
-      <c r="C211">
-        <v>3</v>
-      </c>
-      <c r="D211">
-        <v>4</v>
-      </c>
-      <c r="E211">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A212">
-        <f t="shared" si="3"/>
-        <v>211</v>
-      </c>
-      <c r="B212">
-        <v>4</v>
-      </c>
-      <c r="C212">
-        <v>5</v>
-      </c>
-      <c r="D212">
-        <v>4</v>
-      </c>
-      <c r="E212">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A213">
-        <f t="shared" si="3"/>
-        <v>212</v>
-      </c>
-      <c r="B213">
-        <v>4</v>
-      </c>
-      <c r="C213">
-        <v>7</v>
-      </c>
-      <c r="D213">
-        <v>4</v>
-      </c>
-      <c r="E213">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A214">
-        <f t="shared" si="3"/>
-        <v>213</v>
-      </c>
-      <c r="B214">
-        <v>4</v>
-      </c>
-      <c r="C214">
-        <v>10</v>
-      </c>
-      <c r="D214">
-        <v>4</v>
-      </c>
-      <c r="E214">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A215">
-        <f t="shared" si="3"/>
-        <v>214</v>
-      </c>
-      <c r="B215">
-        <v>4</v>
-      </c>
-      <c r="C215">
-        <v>0</v>
-      </c>
-      <c r="D215">
-        <v>0</v>
-      </c>
-      <c r="E215">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A216">
-        <f t="shared" si="3"/>
-        <v>215</v>
-      </c>
-      <c r="B216">
-        <v>4</v>
-      </c>
-      <c r="C216">
-        <v>2</v>
-      </c>
-      <c r="D216">
-        <v>0</v>
-      </c>
-      <c r="E216">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A217">
-        <f t="shared" si="3"/>
-        <v>216</v>
-      </c>
-      <c r="B217">
-        <v>4</v>
-      </c>
-      <c r="C217">
-        <v>3</v>
-      </c>
-      <c r="D217">
-        <v>0</v>
-      </c>
-      <c r="E217">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A218">
-        <f t="shared" si="3"/>
-        <v>217</v>
-      </c>
-      <c r="B218">
-        <v>4</v>
-      </c>
-      <c r="C218">
-        <v>5</v>
-      </c>
-      <c r="D218">
-        <v>0</v>
-      </c>
-      <c r="E218">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A219">
-        <f t="shared" si="3"/>
-        <v>218</v>
-      </c>
-      <c r="B219">
-        <v>4</v>
-      </c>
-      <c r="C219">
-        <v>7</v>
-      </c>
-      <c r="D219">
-        <v>0</v>
-      </c>
-      <c r="E219">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A220">
-        <f t="shared" si="3"/>
-        <v>219</v>
-      </c>
-      <c r="B220">
-        <v>4</v>
-      </c>
-      <c r="C220">
-        <v>10</v>
-      </c>
-      <c r="D220">
-        <v>0</v>
-      </c>
-      <c r="E220">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A221">
-        <f t="shared" si="3"/>
-        <v>220</v>
-      </c>
-      <c r="B221">
-        <v>4</v>
-      </c>
-      <c r="C221">
-        <v>0</v>
-      </c>
-      <c r="D221">
-        <v>1</v>
-      </c>
-      <c r="E221">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A222">
-        <f t="shared" si="3"/>
-        <v>221</v>
-      </c>
-      <c r="B222">
-        <v>4</v>
-      </c>
-      <c r="C222">
-        <v>2</v>
-      </c>
-      <c r="D222">
-        <v>1</v>
-      </c>
-      <c r="E222">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A223">
-        <f t="shared" si="3"/>
-        <v>222</v>
-      </c>
-      <c r="B223">
-        <v>4</v>
-      </c>
-      <c r="C223">
-        <v>3</v>
-      </c>
-      <c r="D223">
-        <v>1</v>
-      </c>
-      <c r="E223">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A224">
-        <f t="shared" si="3"/>
-        <v>223</v>
-      </c>
-      <c r="B224">
-        <v>4</v>
-      </c>
-      <c r="C224">
-        <v>5</v>
-      </c>
-      <c r="D224">
-        <v>1</v>
-      </c>
-      <c r="E224">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A225">
-        <f t="shared" si="3"/>
-        <v>224</v>
-      </c>
-      <c r="B225">
-        <v>4</v>
-      </c>
-      <c r="C225">
-        <v>7</v>
-      </c>
-      <c r="D225">
-        <v>1</v>
-      </c>
-      <c r="E225">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A226">
-        <f t="shared" si="3"/>
-        <v>225</v>
-      </c>
-      <c r="B226">
-        <v>4</v>
-      </c>
-      <c r="C226">
-        <v>10</v>
-      </c>
-      <c r="D226">
-        <v>1</v>
-      </c>
-      <c r="E226">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A227">
-        <f t="shared" si="3"/>
-        <v>226</v>
-      </c>
-      <c r="B227">
-        <v>4</v>
-      </c>
-      <c r="C227">
-        <v>0</v>
-      </c>
-      <c r="D227">
-        <v>2</v>
-      </c>
-      <c r="E227">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A228">
-        <f t="shared" si="3"/>
-        <v>227</v>
-      </c>
-      <c r="B228">
-        <v>4</v>
-      </c>
-      <c r="C228">
-        <v>2</v>
-      </c>
-      <c r="D228">
-        <v>2</v>
-      </c>
-      <c r="E228">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A229">
-        <f t="shared" si="3"/>
-        <v>228</v>
-      </c>
-      <c r="B229">
-        <v>4</v>
-      </c>
-      <c r="C229">
-        <v>3</v>
-      </c>
-      <c r="D229">
-        <v>2</v>
-      </c>
-      <c r="E229">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A230">
-        <f t="shared" si="3"/>
-        <v>229</v>
-      </c>
-      <c r="B230">
-        <v>4</v>
-      </c>
-      <c r="C230">
-        <v>5</v>
-      </c>
-      <c r="D230">
-        <v>2</v>
-      </c>
-      <c r="E230">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A231">
-        <f t="shared" si="3"/>
-        <v>230</v>
-      </c>
-      <c r="B231">
-        <v>4</v>
-      </c>
-      <c r="C231">
-        <v>7</v>
-      </c>
-      <c r="D231">
-        <v>2</v>
-      </c>
-      <c r="E231">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A232">
-        <f t="shared" si="3"/>
-        <v>231</v>
-      </c>
-      <c r="B232">
-        <v>4</v>
-      </c>
-      <c r="C232">
-        <v>10</v>
-      </c>
-      <c r="D232">
-        <v>2</v>
-      </c>
-      <c r="E232">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A233">
-        <f t="shared" si="3"/>
-        <v>232</v>
-      </c>
-      <c r="B233">
-        <v>4</v>
-      </c>
-      <c r="C233">
-        <v>0</v>
-      </c>
-      <c r="D233">
-        <v>3</v>
-      </c>
-      <c r="E233">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A234">
-        <f t="shared" si="3"/>
-        <v>233</v>
-      </c>
-      <c r="B234">
-        <v>4</v>
-      </c>
-      <c r="C234">
-        <v>2</v>
-      </c>
-      <c r="D234">
-        <v>3</v>
-      </c>
-      <c r="E234">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A235">
-        <f t="shared" si="3"/>
-        <v>234</v>
-      </c>
-      <c r="B235">
-        <v>4</v>
-      </c>
-      <c r="C235">
-        <v>3</v>
-      </c>
-      <c r="D235">
-        <v>3</v>
-      </c>
-      <c r="E235">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A236">
-        <f t="shared" si="3"/>
-        <v>235</v>
-      </c>
-      <c r="B236">
-        <v>4</v>
-      </c>
-      <c r="C236">
-        <v>5</v>
-      </c>
-      <c r="D236">
-        <v>3</v>
-      </c>
-      <c r="E236">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A237">
-        <f t="shared" si="3"/>
-        <v>236</v>
-      </c>
-      <c r="B237">
-        <v>4</v>
-      </c>
-      <c r="C237">
-        <v>7</v>
-      </c>
-      <c r="D237">
-        <v>3</v>
-      </c>
-      <c r="E237">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A238">
-        <f t="shared" si="3"/>
-        <v>237</v>
-      </c>
-      <c r="B238">
-        <v>4</v>
-      </c>
-      <c r="C238">
-        <v>10</v>
-      </c>
-      <c r="D238">
-        <v>3</v>
-      </c>
-      <c r="E238">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A239">
-        <f t="shared" si="3"/>
-        <v>238</v>
-      </c>
-      <c r="B239">
-        <v>4</v>
-      </c>
-      <c r="C239">
-        <v>0</v>
-      </c>
-      <c r="D239">
-        <v>4</v>
-      </c>
-      <c r="E239">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A240">
-        <f t="shared" si="3"/>
-        <v>239</v>
-      </c>
-      <c r="B240">
-        <v>4</v>
-      </c>
-      <c r="C240">
-        <v>2</v>
-      </c>
-      <c r="D240">
-        <v>4</v>
-      </c>
-      <c r="E240">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A241">
-        <f t="shared" si="3"/>
-        <v>240</v>
-      </c>
-      <c r="B241">
-        <v>4</v>
-      </c>
-      <c r="C241">
-        <v>3</v>
-      </c>
-      <c r="D241">
-        <v>4</v>
-      </c>
-      <c r="E241">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A242">
-        <f t="shared" si="3"/>
-        <v>241</v>
-      </c>
-      <c r="B242">
-        <v>4</v>
-      </c>
-      <c r="C242">
-        <v>5</v>
-      </c>
-      <c r="D242">
-        <v>4</v>
-      </c>
-      <c r="E242">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A243">
-        <f t="shared" si="3"/>
-        <v>242</v>
-      </c>
-      <c r="B243">
-        <v>4</v>
-      </c>
-      <c r="C243">
-        <v>7</v>
-      </c>
-      <c r="D243">
-        <v>4</v>
-      </c>
-      <c r="E243">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A244">
-        <f t="shared" si="3"/>
-        <v>243</v>
-      </c>
-      <c r="B244">
-        <v>4</v>
-      </c>
-      <c r="C244">
-        <v>10</v>
-      </c>
-      <c r="D244">
-        <v>4</v>
-      </c>
-      <c r="E244">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A245">
-        <v>244</v>
-      </c>
-      <c r="B245">
-        <v>5</v>
-      </c>
-      <c r="C245">
-        <v>-1</v>
-      </c>
-      <c r="D245">
-        <v>-1</v>
-      </c>
-      <c r="E245">
         <v>-1</v>
       </c>
     </row>

</xml_diff>